<commit_message>
🐞Fix:Fixed display swipe video progress bar(修复显示刷视频进度条)
</commit_message>
<xml_diff>
--- a/answer/国际商务谈判第五期测验作业考试.xlsx
+++ b/answer/国际商务谈判第五期测验作业考试.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\pc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitpush\sk2\answer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A881AF9-4BE4-4B02-8B74-1C380511A2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16129A07-CDA8-4E9D-A374-E756BA124D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15150" yWindow="0" windowWidth="13875" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="答案" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -498,61 +490,62 @@
     <t>20220911084418711506</t>
   </si>
   <si>
+    <t>20220911083425215712</t>
+  </si>
+  <si>
+    <t>国际商务谈判的概念 </t>
+  </si>
+  <si>
+    <t>20220911012911391975</t>
+  </si>
+  <si>
+    <t>国际商务谈判的特点测试 </t>
+  </si>
+  <si>
+    <t>20220912175723763625</t>
+  </si>
+  <si>
+    <t>素质拓展篇作业 </t>
+  </si>
+  <si>
+    <t>20220912175121503283</t>
+  </si>
+  <si>
+    <t>情境创设篇作业 </t>
+  </si>
+  <si>
+    <t>20220912174647218720</t>
+  </si>
+  <si>
+    <t>项目实践篇作业 </t>
+  </si>
+  <si>
+    <t>20220912173434757376</t>
+  </si>
+  <si>
+    <t>基础理论篇作业 </t>
+  </si>
+  <si>
+    <t>20220911000354855762</t>
+  </si>
+  <si>
+    <t>国际商务谈判期末考试（第五次开课） </t>
+  </si>
+  <si>
+    <t>课程满意度调查问卷 </t>
+  </si>
+  <si>
+    <t>“一带一路”：构建人类命运共同体测试 </t>
+  </si>
+  <si>
+    <t>日常交往重细节—谈判日常礼仪测试 </t>
+  </si>
+  <si>
+    <t>觥筹交错知进退—谈判宴请礼仪测试 </t>
+  </si>
+  <si>
     <t>国际商务谈判的种类测试 </t>
-  </si>
-  <si>
-    <t>20220911083425215712</t>
-  </si>
-  <si>
-    <t>国际商务谈判的概念 </t>
-  </si>
-  <si>
-    <t>20220911012911391975</t>
-  </si>
-  <si>
-    <t>国际商务谈判的特点测试 </t>
-  </si>
-  <si>
-    <t>20220912175723763625</t>
-  </si>
-  <si>
-    <t>素质拓展篇作业 </t>
-  </si>
-  <si>
-    <t>20220912175121503283</t>
-  </si>
-  <si>
-    <t>情境创设篇作业 </t>
-  </si>
-  <si>
-    <t>20220912174647218720</t>
-  </si>
-  <si>
-    <t>项目实践篇作业 </t>
-  </si>
-  <si>
-    <t>20220912173434757376</t>
-  </si>
-  <si>
-    <t>基础理论篇作业 </t>
-  </si>
-  <si>
-    <t>20220911000354855762</t>
-  </si>
-  <si>
-    <t>国际商务谈判期末考试（第五次开课） </t>
-  </si>
-  <si>
-    <t>课程满意度调查问卷 </t>
-  </si>
-  <si>
-    <t>“一带一路”：构建人类命运共同体测试 </t>
-  </si>
-  <si>
-    <t>日常交往重细节—谈判日常礼仪测试 </t>
-  </si>
-  <si>
-    <t>觥筹交错知进退—谈判宴请礼仪测试 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -595,12 +588,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -885,19 +875,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:ET69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O69" sqref="O69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.75" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.75" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1055,11 +1045,11 @@
       </c>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -1081,11 +1071,11 @@
       </c>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -1107,11 +1097,11 @@
       </c>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>
@@ -1154,11 +1144,11 @@
       </c>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -1198,7 +1188,7 @@
       </c>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1356,7 +1346,7 @@
       </c>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1514,7 +1504,7 @@
       </c>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1672,7 +1662,7 @@
       </c>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1830,7 +1820,7 @@
       </c>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1988,7 +1978,7 @@
       </c>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2146,7 +2136,7 @@
       </c>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2304,7 +2294,7 @@
       </c>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2462,7 +2452,7 @@
       </c>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2620,7 +2610,7 @@
       </c>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -2778,7 +2768,7 @@
       </c>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2936,7 +2926,7 @@
       </c>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3094,7 +3084,7 @@
       </c>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -3252,7 +3242,7 @@
       </c>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -3410,7 +3400,7 @@
       </c>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -3568,7 +3558,7 @@
       </c>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3726,7 +3716,7 @@
       </c>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3884,7 +3874,7 @@
       </c>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -4042,7 +4032,7 @@
       </c>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -4200,7 +4190,7 @@
       </c>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -4358,7 +4348,7 @@
       </c>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -4516,7 +4506,7 @@
       </c>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -4674,7 +4664,7 @@
       </c>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -4832,7 +4822,7 @@
       </c>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -4990,7 +4980,7 @@
       </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -5148,7 +5138,7 @@
       </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -5306,7 +5296,7 @@
       </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -5464,7 +5454,7 @@
       </c>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -5622,7 +5612,7 @@
       </c>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -5780,7 +5770,7 @@
       </c>
     </row>
     <row r="35" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -5938,7 +5928,7 @@
       </c>
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -6096,7 +6086,7 @@
       </c>
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -6254,7 +6244,7 @@
       </c>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -6412,7 +6402,7 @@
       </c>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -6570,7 +6560,7 @@
       </c>
     </row>
     <row r="40" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -6728,7 +6718,7 @@
       </c>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -6886,7 +6876,7 @@
       </c>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -7044,7 +7034,7 @@
       </c>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -7202,7 +7192,7 @@
       </c>
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -7360,7 +7350,7 @@
       </c>
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -7518,7 +7508,7 @@
       </c>
     </row>
     <row r="46" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -7676,7 +7666,7 @@
       </c>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -7834,7 +7824,7 @@
       </c>
     </row>
     <row r="48" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -7992,7 +7982,7 @@
       </c>
     </row>
     <row r="49" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -8150,7 +8140,7 @@
       </c>
     </row>
     <row r="50" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -8308,7 +8298,7 @@
       </c>
     </row>
     <row r="51" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>129</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -8466,7 +8456,7 @@
       </c>
     </row>
     <row r="52" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>132</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -8624,7 +8614,7 @@
       </c>
     </row>
     <row r="53" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -8782,7 +8772,7 @@
       </c>
     </row>
     <row r="54" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>136</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -8940,7 +8930,7 @@
       </c>
     </row>
     <row r="55" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>138</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -9098,7 +9088,7 @@
       </c>
     </row>
     <row r="56" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -9256,7 +9246,7 @@
       </c>
     </row>
     <row r="57" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -9414,7 +9404,7 @@
       </c>
     </row>
     <row r="58" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -9572,7 +9562,7 @@
       </c>
     </row>
     <row r="59" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>146</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -9730,11 +9720,11 @@
       </c>
     </row>
     <row r="60" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>10</v>
@@ -9888,11 +9878,11 @@
       </c>
     </row>
     <row r="61" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>72</v>
@@ -10046,11 +10036,11 @@
       </c>
     </row>
     <row r="62" spans="1:150" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>21</v>
@@ -10205,10 +10195,10 @@
     </row>
     <row r="64" spans="1:150" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" t="s">
         <v>155</v>
-      </c>
-      <c r="B64" t="s">
-        <v>156</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>3</v>
@@ -10657,10 +10647,10 @@
     </row>
     <row r="65" spans="1:150" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>156</v>
+      </c>
+      <c r="B65" t="s">
         <v>157</v>
-      </c>
-      <c r="B65" t="s">
-        <v>158</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>14</v>
@@ -11109,10 +11099,10 @@
     </row>
     <row r="66" spans="1:150" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>158</v>
+      </c>
+      <c r="B66" t="s">
         <v>159</v>
-      </c>
-      <c r="B66" t="s">
-        <v>160</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>23</v>
@@ -11561,10 +11551,10 @@
     </row>
     <row r="67" spans="1:150" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>160</v>
+      </c>
+      <c r="B67" t="s">
         <v>161</v>
-      </c>
-      <c r="B67" t="s">
-        <v>162</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>23</v>
@@ -12013,10 +12003,10 @@
     </row>
     <row r="69" spans="1:150" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>162</v>
+      </c>
+      <c r="B69" t="s">
         <v>163</v>
-      </c>
-      <c r="B69" t="s">
-        <v>164</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>12</v>

</xml_diff>